<commit_message>
Modificacion sobre concentrado de metricas Marzo
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150331.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150331.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="2"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -224,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +264,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +467,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -478,9 +502,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -534,17 +555,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1100,6 +1143,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1170,10 +1214,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>140</c:v>
+                  <c:v>91.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45.600000000000009</c:v>
@@ -1298,11 +1342,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4488368"/>
-        <c:axId val="4488928"/>
+        <c:axId val="290175120"/>
+        <c:axId val="290175680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4488368"/>
+        <c:axId val="290175120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1356,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4488928"/>
+        <c:crossAx val="290175680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1320,7 +1364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4488928"/>
+        <c:axId val="290175680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1331,13 +1375,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4488368"/>
+        <c:crossAx val="290175120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1445,11 +1490,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="176901840"/>
-        <c:axId val="176902400"/>
+        <c:axId val="154350800"/>
+        <c:axId val="154351360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="176901840"/>
+        <c:axId val="154350800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1504,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176902400"/>
+        <c:crossAx val="154351360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1467,7 +1512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176902400"/>
+        <c:axId val="154351360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1479,7 +1524,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176901840"/>
+        <c:crossAx val="154350800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1537,6 +1582,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1657,11 +1703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="176905760"/>
-        <c:axId val="176906320"/>
+        <c:axId val="288226112"/>
+        <c:axId val="288226672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="176905760"/>
+        <c:axId val="288226112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1717,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176906320"/>
+        <c:crossAx val="288226672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1679,7 +1725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176906320"/>
+        <c:axId val="288226672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1691,7 +1737,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176905760"/>
+        <c:crossAx val="288226112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1744,6 +1790,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1814,10 +1861,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.77857142857142858</c:v>
+                  <c:v>0.66008771929824561</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93571428571428572</c:v>
+                  <c:v>0.80263157894736847</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.34210526315789486</c:v>
@@ -1852,11 +1899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4491728"/>
-        <c:axId val="4492288"/>
+        <c:axId val="291409632"/>
+        <c:axId val="291410192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4491728"/>
+        <c:axId val="291409632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1866,7 +1913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4492288"/>
+        <c:crossAx val="291410192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1874,7 +1921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4492288"/>
+        <c:axId val="291410192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1887,7 +1934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4491728"/>
+        <c:crossAx val="291409632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1980,7 +2027,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11653</c:v>
+                  <c:v>9989</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5693.7300000000005</c:v>
@@ -2030,7 +2077,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4329.6000000000004</c:v>
+                  <c:v>1664.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3123.4</c:v>
@@ -2053,11 +2100,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151480176"/>
-        <c:axId val="151480736"/>
+        <c:axId val="291412992"/>
+        <c:axId val="398043664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151480176"/>
+        <c:axId val="291412992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,7 +2114,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151480736"/>
+        <c:crossAx val="398043664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2075,7 +2122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151480736"/>
+        <c:axId val="398043664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2086,7 +2133,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151480176"/>
+        <c:crossAx val="291412992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2184,7 +2231,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.6284561915386595</c:v>
+                  <c:v>0.83333667033737113</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.45143166254810119</c:v>
@@ -2207,11 +2254,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151483536"/>
-        <c:axId val="151484096"/>
+        <c:axId val="398046464"/>
+        <c:axId val="398047024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151483536"/>
+        <c:axId val="398046464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151484096"/>
+        <c:crossAx val="398047024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2229,7 +2276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151484096"/>
+        <c:axId val="398047024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2242,7 +2289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151483536"/>
+        <c:crossAx val="398046464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2353,11 +2400,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151243488"/>
-        <c:axId val="151244048"/>
+        <c:axId val="314058848"/>
+        <c:axId val="314059408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151243488"/>
+        <c:axId val="314058848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,7 +2414,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151244048"/>
+        <c:crossAx val="314059408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2375,7 +2422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151244048"/>
+        <c:axId val="314059408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2386,7 +2433,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151243488"/>
+        <c:crossAx val="314058848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2503,11 +2550,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151246848"/>
-        <c:axId val="151247408"/>
+        <c:axId val="153284928"/>
+        <c:axId val="153285488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151246848"/>
+        <c:axId val="153284928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2517,7 +2564,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151247408"/>
+        <c:crossAx val="153285488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2525,7 +2572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151247408"/>
+        <c:axId val="153285488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2537,7 +2584,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151246848"/>
+        <c:crossAx val="153284928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2590,7 +2637,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2660,11 +2706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151250208"/>
-        <c:axId val="151250768"/>
+        <c:axId val="293554272"/>
+        <c:axId val="293554832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151250208"/>
+        <c:axId val="293554272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2674,7 +2720,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151250768"/>
+        <c:crossAx val="293554832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2682,7 +2728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151250768"/>
+        <c:axId val="293554832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2694,7 +2740,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151250208"/>
+        <c:crossAx val="293554272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2747,7 +2793,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2811,11 +2856,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101426928"/>
-        <c:axId val="101427488"/>
+        <c:axId val="398911680"/>
+        <c:axId val="398912240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101426928"/>
+        <c:axId val="398911680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2825,7 +2870,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101427488"/>
+        <c:crossAx val="398912240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2833,7 +2878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101427488"/>
+        <c:axId val="398912240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2845,7 +2890,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101426928"/>
+        <c:crossAx val="398911680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2961,11 +3006,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101430288"/>
-        <c:axId val="101430848"/>
+        <c:axId val="398915040"/>
+        <c:axId val="154348000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101430288"/>
+        <c:axId val="398915040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,7 +3020,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101430848"/>
+        <c:crossAx val="154348000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2983,7 +3028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101430848"/>
+        <c:axId val="154348000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2995,7 +3040,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101430288"/>
+        <c:crossAx val="398915040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3742,8 +3787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3779,131 +3824,131 @@
     <row r="17" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="39">
-        <v>140</v>
-      </c>
-      <c r="E20" s="39">
+      <c r="D20" s="37">
+        <v>91.2</v>
+      </c>
+      <c r="E20" s="37">
         <v>31</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="42">
         <f>(D20-E20)/D20</f>
-        <v>0.77857142857142858</v>
+        <v>0.66008771929824561</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="39">
-        <v>140</v>
-      </c>
-      <c r="E21" s="39">
+      <c r="D21" s="37">
+        <v>45.6</v>
+      </c>
+      <c r="E21" s="37">
         <v>9</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="42">
         <f t="shared" ref="F21:F23" si="0">(D21-E21)/D21</f>
-        <v>0.93571428571428572</v>
+        <v>0.80263157894736847</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="37">
         <v>45.600000000000009</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E22" s="37">
         <v>30</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="43">
         <f t="shared" si="0"/>
         <v>0.34210526315789486</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="50"/>
+      <c r="C23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="37">
         <v>91.200000000000017</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="37">
         <v>40</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="43">
         <f t="shared" si="0"/>
         <v>0.5614035087719299</v>
       </c>
     </row>
     <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36">
+      <c r="C24" s="36"/>
+      <c r="D24" s="35">
         <v>1</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="35">
         <v>1</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="44">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="36">
+      <c r="C25" s="36"/>
+      <c r="D25" s="35">
         <v>2</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="35">
         <v>1.6</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="44">
         <f t="shared" ref="F25:F26" si="1">(D25-E25)/D25</f>
         <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36">
+      <c r="C26" s="36"/>
+      <c r="D26" s="35">
         <v>0.5</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="39">
         <v>0.17</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="45">
         <f t="shared" si="1"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4411,8 +4456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4466,14 +4511,14 @@
         <v>4</v>
       </c>
       <c r="C20" s="15">
-        <v>11653</v>
+        <v>9989</v>
       </c>
       <c r="D20" s="15">
-        <v>4329.6000000000004</v>
-      </c>
-      <c r="E20" s="16">
+        <v>1664.8</v>
+      </c>
+      <c r="E20" s="40">
         <f>(C20-D20)/C20</f>
-        <v>0.6284561915386595</v>
+        <v>0.83333667033737113</v>
       </c>
     </row>
     <row r="21" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4486,7 +4531,7 @@
       <c r="D21" s="15">
         <v>3123.4</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="41">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.45143166254810119</v>
       </c>
@@ -4518,8 +4563,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4539,94 +4584,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="48">
         <v>1</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="48">
         <v>1</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="49">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="48">
         <v>0.8</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="49">
         <f>AVERAGE(D5:F5)</f>
         <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="26" t="e">
+      <c r="G6" s="25" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4636,91 +4681,91 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="30">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="29">
         <v>150227</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>150331</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="26"/>
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="28" t="e">
+      <c r="F10" s="23"/>
+      <c r="G10" s="27" t="e">
         <f t="shared" ref="G10:G12" si="0">AVERAGE(D10:F10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="28" t="e">
+      <c r="F11" s="23"/>
+      <c r="G11" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="28" t="e">
+      <c r="F12" s="23"/>
+      <c r="G12" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -4812,8 +4857,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,56 +4876,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="47">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="47">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4888,22 +4933,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="47">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="47">
         <v>1</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -4911,22 +4956,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="47">
         <v>1</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="47">
         <v>1</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="46">
         <f>AVERAGE(D6:F6)</f>
         <v>1</v>
       </c>
@@ -4934,22 +4979,22 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="47">
         <v>1</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="46">
         <f>AVERAGE(D7:F7)</f>
         <v>1</v>
       </c>
@@ -4957,67 +5002,67 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="30">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="29">
         <v>150227</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>150331</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>1</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="26" t="e">
+      <c r="G11" s="25" t="e">
         <f t="shared" ref="G11:G13" si="0">AVERAGE(D11:F11)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5025,22 +5070,22 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="26" t="e">
+      <c r="G12" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5048,22 +5093,22 @@
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="26" t="e">
+      <c r="G13" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5229,7 +5274,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="D4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5247,56 +5292,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="47">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="47">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5304,22 +5349,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="47">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="47">
         <v>1</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5327,22 +5372,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="28" t="e">
+      <c r="G6" s="27" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5432,7 +5477,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,56 +5495,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>0.75</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>0.875</v>
       </c>
@@ -5507,22 +5552,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5530,22 +5575,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="28" t="e">
+      <c r="G6" s="27" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5635,7 +5680,7 @@
   <dimension ref="C2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5646,77 +5691,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="30">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="29">
         <v>150227</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150331</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>2</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>